<commit_message>
Extracted Coefficients for the best models.
</commit_message>
<xml_diff>
--- a/Analysis/Tables/TableX_Shrinkage.xlsx
+++ b/Analysis/Tables/TableX_Shrinkage.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Table X The averaged coefficients of the predictor variables included in the best subset of models as in Table X. Calculated with shrinkage. NA: parameter was not included in the models</t>
   </si>
@@ -194,18 +194,6 @@
       </rPr>
       <t xml:space="preserve"> x SamCam 3</t>
     </r>
-  </si>
-  <si>
-    <t>Model R²</t>
-  </si>
-  <si>
-    <t>Family</t>
-  </si>
-  <si>
-    <t>Poisson</t>
-  </si>
-  <si>
-    <t>Log-Normal</t>
   </si>
 </sst>
 </file>
@@ -272,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -285,6 +273,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -586,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L41"/>
+  <dimension ref="B2:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1043,54 +1032,22 @@
         <v>3.6339711298131301E-2</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
+    <row r="37" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="2">
+      <c r="C37" s="7"/>
+      <c r="D37" s="8">
         <v>3.4300744714824097E-2</v>
       </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C38" s="3"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C39" s="3"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="2">
-        <v>0.71399999999999997</v>
-      </c>
-      <c r="D40" s="2">
-        <v>0.61699999999999999</v>
-      </c>
-      <c r="E40" s="3">
-        <v>0.35299999999999998</v>
-      </c>
-      <c r="F40">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>34</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>